<commit_message>
Sertifikat Done, RBAC Implemented, Buff Folder Drop, Osyawwal Drop change to Osyawwal with Default Data
</commit_message>
<xml_diff>
--- a/file/template/pusdiklat/evaluation/certificate.receipt.xlsx
+++ b/file/template/pusdiklat/evaluation/certificate.receipt.xlsx
@@ -202,14 +202,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,7 +564,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,14 +586,14 @@
       <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
@@ -612,30 +612,30 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="20"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="17"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -668,7 +668,7 @@
       </c>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="13"/>
       <c r="C12" s="5"/>

</xml_diff>